<commit_message>
loads of bug fixes
</commit_message>
<xml_diff>
--- a/algorithm_list.xlsx
+++ b/algorithm_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayukikishi/Dropbox (Personal)/masayuki_kishi/repositories/create_names/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2462BA94-BEC8-A241-8D0E-025D1574EAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E833713-8432-DB4E-A597-93371638D996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29860" windowHeight="17160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29860" windowHeight="17160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2_word_algorithm" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
   <si>
     <t>keyword_type_1</t>
   </si>
@@ -572,7 +572,7 @@
   <dimension ref="A1:AMJ10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -635,7 +635,9 @@
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -648,7 +650,9 @@
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -661,7 +665,9 @@
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -676,7 +682,9 @@
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -691,7 +699,9 @@
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -721,7 +731,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:E9 A10">
+  <conditionalFormatting sqref="A1:E3 A10 A9:E9 A4:D8">
     <cfRule type="expression" dxfId="4" priority="2">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>

</xml_diff>